<commit_message>
Change test names in create computer
</commit_message>
<xml_diff>
--- a/resources/CRUD TestCases.xlsx
+++ b/resources/CRUD TestCases.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21727"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A37FB507-B889-474B-A358-5A58C07EAD97}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC0C9108-7A25-435A-974D-D20225F242CD}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -166,25 +166,6 @@
 3- Use (IE,Google Chrome ,Fire Fox)
 4- All fields of the computer are mandatory
 5- I make manual test for search computer function and it work well so i use it to verify that computer was created and appear in the list </t>
-  </si>
-  <si>
-    <t>1- Number of computer appear with number for example "270"
-2- Home page opened with a list of previous created computers with these fields (computer name , introduced date, disconnected date , company )
-3- Add new computer button appear in Home screen
-4- Total number of computers appear on the top left
-5- Add new computer opened with these fields :c
-computer name as text box
-introduced date as text box with specific format "yyyy-mm-dd"
-disconnected date : as text box with specific format "yyyy-mm-dd
-company : drop down list with specific names inside 
-6- Create computer button appear 
-7- Cancel button appear 
-8- User navigate to home page 
-9- New computer created with success message appear on the top of the list of computer 
-10- Computer appear in list of the created computer after make search and all entered values appear  in the fields 
-11- Date appear with this format 
-"DD MMM YYYY"
-12- Number of computers increased plus one</t>
   </si>
   <si>
     <t xml:space="preserve">Highest </t>
@@ -636,12 +617,31 @@
     <t>1- Computer should be created successfully with all entered data 
 2- Number of computers will be increased +1</t>
   </si>
+  <si>
+    <t>1- Number of computer appear with number for example "270"
+2- Home page opened with a list of previous created computers with these fields (computer name , introduced date, disconnected date , company )
+3- Add new computer button appear in Home screen
+4- Total number of computers appear on the top left
+5- Add new computer opened with these fields :c
+computer name as text box
+introduced date as text box with specific format "yyyy-mm-dd"
+disconnected date : as text box with specific format "yyyy-mm-dd
+company : drop down list with specific names inside 
+6- Create computer button appear 
+7- Cancel button appear 
+8- User navigate to home page 
+9- New computer created with success message appear on the top of the list of computer 
+10- Computer appear in list of the created computer after make search and all entered values appear  in the fields 
+11- Date appear with this format 
+"DD MMM YYYY"
+12- Number of computers increased plus one</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="15" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -676,13 +676,6 @@
       <family val="2"/>
     </font>
     <font>
-      <b/>
-      <sz val="8"/>
-      <color indexed="8"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
       <sz val="10"/>
       <name val="Verdana"/>
       <family val="2"/>
@@ -694,12 +687,6 @@
     </font>
     <font>
       <sz val="9"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color indexed="8"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -816,111 +803,75 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="14" fontId="8" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -929,11 +880,17 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="7" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1215,860 +1172,792 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I40"/>
+  <dimension ref="A1:I34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="H22" sqref="H22"/>
+    <sheetView tabSelected="1" topLeftCell="A32" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="D36" sqref="D36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.28515625" style="24" customWidth="1"/>
-    <col min="2" max="2" width="30" style="36" customWidth="1"/>
-    <col min="3" max="3" width="32.85546875" style="24" customWidth="1"/>
-    <col min="4" max="4" width="26.140625" style="33" customWidth="1"/>
-    <col min="5" max="5" width="26.140625" style="24" customWidth="1"/>
-    <col min="6" max="6" width="32.85546875" style="24" customWidth="1"/>
-    <col min="7" max="7" width="14.42578125" style="24" customWidth="1"/>
-    <col min="8" max="8" width="13.5703125" style="24" customWidth="1"/>
-    <col min="9" max="16384" width="9.140625" style="24"/>
+    <col min="1" max="1" width="18.28515625" style="18" customWidth="1"/>
+    <col min="2" max="2" width="30" style="24" customWidth="1"/>
+    <col min="3" max="3" width="32.85546875" style="18" customWidth="1"/>
+    <col min="4" max="4" width="26.140625" style="21" customWidth="1"/>
+    <col min="5" max="5" width="26.140625" style="18" customWidth="1"/>
+    <col min="6" max="6" width="32.85546875" style="31" customWidth="1"/>
+    <col min="7" max="7" width="14.42578125" style="18" customWidth="1"/>
+    <col min="8" max="8" width="13.5703125" style="18" customWidth="1"/>
+    <col min="9" max="16384" width="9.140625" style="18"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="38"/>
-      <c r="B1" s="34" t="s">
+      <c r="A1" s="26"/>
+      <c r="B1" s="22" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="5"/>
-      <c r="D1" s="31" t="s">
+      <c r="D1" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="21" t="s">
+      <c r="E1" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="F1" s="22"/>
+      <c r="F1" s="28"/>
       <c r="G1" s="2"/>
       <c r="H1" s="3"/>
       <c r="I1" s="4"/>
     </row>
     <row r="2" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="39"/>
-      <c r="B2" s="22" t="s">
+      <c r="A2" s="27"/>
+      <c r="B2" s="17" t="s">
         <v>2</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="D2" s="31" t="s">
+      <c r="D2" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="21"/>
-      <c r="F2" s="25"/>
+      <c r="E2" s="16"/>
+      <c r="F2" s="29"/>
       <c r="G2" s="2"/>
       <c r="H2" s="3"/>
       <c r="I2" s="4"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="28"/>
-      <c r="B3" s="7"/>
-      <c r="C3" s="8"/>
-      <c r="D3" s="32"/>
-      <c r="E3" s="7"/>
-      <c r="F3" s="26"/>
-      <c r="G3" s="2"/>
-      <c r="H3" s="3"/>
-      <c r="I3" s="4"/>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="28"/>
-      <c r="B4" s="7"/>
-      <c r="C4" s="8"/>
-      <c r="D4" s="32"/>
-      <c r="E4" s="7"/>
-      <c r="F4" s="27"/>
-      <c r="G4" s="2"/>
-      <c r="H4" s="3"/>
-      <c r="I4" s="4"/>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="6"/>
-      <c r="B5" s="7"/>
-      <c r="C5" s="7"/>
-      <c r="D5" s="32"/>
-      <c r="E5" s="8"/>
-      <c r="F5" s="7"/>
-      <c r="G5" s="2"/>
-      <c r="H5" s="3"/>
-      <c r="I5" s="8"/>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="6"/>
-      <c r="B6" s="40"/>
-      <c r="C6" s="41"/>
-      <c r="D6" s="41"/>
-      <c r="E6" s="41"/>
-      <c r="F6" s="41"/>
-      <c r="G6" s="41"/>
-      <c r="H6" s="41"/>
-      <c r="I6" s="10"/>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="6"/>
-      <c r="B7" s="40"/>
-      <c r="C7" s="41"/>
-      <c r="D7" s="41"/>
-      <c r="E7" s="41"/>
-      <c r="F7" s="41"/>
-      <c r="G7" s="41"/>
-      <c r="H7" s="41"/>
-      <c r="I7" s="10"/>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="6"/>
-      <c r="B8" s="29"/>
-      <c r="C8" s="23"/>
-      <c r="D8" s="23"/>
-      <c r="E8" s="9"/>
-      <c r="F8" s="23"/>
-      <c r="G8" s="2"/>
-      <c r="H8" s="3"/>
-      <c r="I8" s="10"/>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="13"/>
-      <c r="B9" s="14"/>
-      <c r="C9" s="14"/>
-      <c r="D9" s="14"/>
-      <c r="E9" s="15"/>
-      <c r="F9" s="14"/>
-      <c r="G9" s="13"/>
-      <c r="H9" s="13"/>
-      <c r="I9" s="15"/>
-    </row>
-    <row r="10" spans="1:9" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="17" t="s">
+      <c r="A3" s="8"/>
+      <c r="B3" s="9"/>
+      <c r="C3" s="9"/>
+      <c r="D3" s="9"/>
+      <c r="E3" s="10"/>
+      <c r="F3" s="30"/>
+      <c r="G3" s="8"/>
+      <c r="H3" s="8"/>
+      <c r="I3" s="10"/>
+    </row>
+    <row r="4" spans="1:9" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="B10" s="18" t="s">
+      <c r="B4" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="C10" s="17" t="s">
+      <c r="C4" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="D10" s="16" t="s">
+      <c r="D4" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="E10" s="17" t="s">
+      <c r="E4" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="F10" s="18" t="s">
+      <c r="F4" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="G10" s="17" t="s">
+      <c r="G4" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="H10" s="17" t="s">
+      <c r="H4" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="I10" s="30"/>
-    </row>
-    <row r="11" spans="1:9" ht="408.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="12">
+      <c r="I4" s="19"/>
+    </row>
+    <row r="5" spans="1:9" ht="409.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="7">
         <v>1</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="B5" s="1" t="s">
         <v>17</v>
       </c>
+      <c r="C5" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="G5" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="H5" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="I5" s="19"/>
+    </row>
+    <row r="6" spans="1:9" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="7">
+        <v>2</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="G6" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="H6" s="6"/>
+      <c r="I6" s="19"/>
+    </row>
+    <row r="7" spans="1:9" ht="216" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="7">
+        <v>3</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="G7" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="H7" s="6"/>
+      <c r="I7" s="19"/>
+    </row>
+    <row r="8" spans="1:9" ht="212.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="7">
+        <v>4</v>
+      </c>
+      <c r="B8" s="23" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="G8" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="H8" s="6"/>
+      <c r="I8" s="19"/>
+    </row>
+    <row r="9" spans="1:9" ht="165" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="7">
+        <v>5</v>
+      </c>
+      <c r="B9" s="23" t="s">
+        <v>47</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E9" s="1"/>
+      <c r="F9" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="G9" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="H9" s="6"/>
+      <c r="I9" s="19"/>
+    </row>
+    <row r="10" spans="1:9" ht="165" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="7">
+        <v>6</v>
+      </c>
+      <c r="B10" s="23" t="s">
+        <v>72</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="G10" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="H10" s="6"/>
+      <c r="I10" s="19"/>
+    </row>
+    <row r="11" spans="1:9" ht="165" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="7">
+        <v>7</v>
+      </c>
+      <c r="B11" s="23" t="s">
+        <v>74</v>
+      </c>
       <c r="C11" s="1" t="s">
-        <v>26</v>
+        <v>88</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>33</v>
-      </c>
+        <v>75</v>
+      </c>
+      <c r="E11" s="1"/>
       <c r="F11" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="G11" s="19" t="s">
-        <v>11</v>
-      </c>
-      <c r="H11" s="11" t="s">
-        <v>35</v>
-      </c>
-      <c r="I11" s="30"/>
-    </row>
-    <row r="12" spans="1:9" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="12">
-        <v>2</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>18</v>
+        <v>76</v>
+      </c>
+      <c r="G11" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="H11" s="6"/>
+      <c r="I11" s="19"/>
+    </row>
+    <row r="12" spans="1:9" ht="165" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="7">
+        <v>8</v>
+      </c>
+      <c r="B12" s="23" t="s">
+        <v>87</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>25</v>
+        <v>89</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>19</v>
-      </c>
+        <v>92</v>
+      </c>
+      <c r="E12" s="1"/>
       <c r="F12" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="G12" s="19" t="s">
-        <v>11</v>
-      </c>
-      <c r="H12" s="11"/>
-      <c r="I12" s="30"/>
-    </row>
-    <row r="13" spans="1:9" ht="216" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="12">
-        <v>3</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>13</v>
+        <v>93</v>
+      </c>
+      <c r="G12" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="H12" s="6"/>
+      <c r="I12" s="19"/>
+    </row>
+    <row r="13" spans="1:9" ht="165" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="7">
+        <v>9</v>
+      </c>
+      <c r="B13" s="23" t="s">
+        <v>91</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>23</v>
+        <v>90</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="E13" s="1" t="s">
-        <v>19</v>
-      </c>
+        <v>92</v>
+      </c>
+      <c r="E13" s="1"/>
       <c r="F13" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="G13" s="19" t="s">
-        <v>11</v>
-      </c>
-      <c r="H13" s="11"/>
-      <c r="I13" s="30"/>
-    </row>
-    <row r="14" spans="1:9" ht="212.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="12">
-        <v>4</v>
-      </c>
-      <c r="B14" s="35" t="s">
-        <v>14</v>
+        <v>93</v>
+      </c>
+      <c r="G13" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="H13" s="6"/>
+      <c r="I13" s="19"/>
+    </row>
+    <row r="14" spans="1:9" ht="210" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="7">
+        <v>10</v>
+      </c>
+      <c r="B14" s="23" t="s">
+        <v>32</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>46</v>
+        <v>61</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>43</v>
+        <v>70</v>
       </c>
       <c r="E14" s="1"/>
       <c r="F14" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="G14" s="19" t="s">
-        <v>45</v>
-      </c>
-      <c r="H14" s="11"/>
-      <c r="I14" s="30"/>
-    </row>
-    <row r="15" spans="1:9" ht="165" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="12">
-        <v>5</v>
-      </c>
-      <c r="B15" s="35" t="s">
-        <v>48</v>
+        <v>69</v>
+      </c>
+      <c r="G14" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="H14" s="6"/>
+      <c r="I14" s="19"/>
+    </row>
+    <row r="15" spans="1:9" ht="217.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="7">
+        <v>11</v>
+      </c>
+      <c r="B15" s="23" t="s">
+        <v>31</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>47</v>
+        <v>62</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>43</v>
+        <v>71</v>
       </c>
       <c r="E15" s="1"/>
       <c r="F15" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="G15" s="19" t="s">
-        <v>45</v>
-      </c>
-      <c r="H15" s="11"/>
-      <c r="I15" s="30"/>
-    </row>
-    <row r="16" spans="1:9" ht="165" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="12">
-        <v>6</v>
-      </c>
-      <c r="B16" s="35" t="s">
-        <v>73</v>
+        <v>68</v>
+      </c>
+      <c r="G15" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="H15" s="6"/>
+      <c r="I15" s="19"/>
+    </row>
+    <row r="16" spans="1:9" ht="176.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="7">
+        <v>12</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>30</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>74</v>
+        <v>63</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>43</v>
+        <v>77</v>
       </c>
       <c r="E16" s="1"/>
       <c r="F16" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="G16" s="19" t="s">
-        <v>45</v>
-      </c>
-      <c r="H16" s="11"/>
-      <c r="I16" s="30"/>
-    </row>
-    <row r="17" spans="1:9" ht="165" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="12">
-        <v>7</v>
-      </c>
-      <c r="B17" s="35" t="s">
-        <v>75</v>
+        <v>110</v>
+      </c>
+      <c r="G16" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="H16" s="6"/>
+      <c r="I16" s="19"/>
+    </row>
+    <row r="17" spans="1:9" ht="133.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="7">
+        <v>13</v>
+      </c>
+      <c r="B17" s="25" t="s">
+        <v>36</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>89</v>
+        <v>64</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="E17" s="1"/>
       <c r="F17" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="G17" s="19" t="s">
-        <v>45</v>
-      </c>
-      <c r="H17" s="11"/>
-      <c r="I17" s="30"/>
-    </row>
-    <row r="18" spans="1:9" ht="165" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="12">
-        <v>8</v>
-      </c>
-      <c r="B18" s="35" t="s">
-        <v>88</v>
+        <v>110</v>
+      </c>
+      <c r="G17" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="H17" s="6"/>
+      <c r="I17" s="19"/>
+    </row>
+    <row r="18" spans="1:9" ht="149.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="7">
+        <v>14</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>29</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>90</v>
+        <v>65</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>93</v>
+        <v>79</v>
       </c>
       <c r="E18" s="1"/>
       <c r="F18" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="G18" s="19" t="s">
-        <v>45</v>
-      </c>
-      <c r="H18" s="11"/>
-      <c r="I18" s="30"/>
-    </row>
-    <row r="19" spans="1:9" ht="165" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="12">
-        <v>9</v>
-      </c>
-      <c r="B19" s="35" t="s">
-        <v>92</v>
+        <v>80</v>
+      </c>
+      <c r="G18" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="H18" s="6"/>
+      <c r="I18" s="19"/>
+    </row>
+    <row r="19" spans="1:9" ht="147.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="7">
+        <v>15</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>28</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>91</v>
+        <v>66</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>93</v>
+        <v>81</v>
       </c>
       <c r="E19" s="1"/>
       <c r="F19" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="G19" s="19" t="s">
-        <v>45</v>
-      </c>
-      <c r="H19" s="11"/>
-      <c r="I19" s="30"/>
-    </row>
-    <row r="20" spans="1:9" ht="210" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="12">
-        <v>10</v>
-      </c>
-      <c r="B20" s="35" t="s">
-        <v>32</v>
+        <v>82</v>
+      </c>
+      <c r="G19" s="15" t="s">
+        <v>83</v>
+      </c>
+      <c r="H19" s="6"/>
+      <c r="I19" s="19"/>
+    </row>
+    <row r="20" spans="1:9" ht="139.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="7">
+        <v>16</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>27</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>62</v>
+        <v>67</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>71</v>
+        <v>84</v>
       </c>
       <c r="E20" s="1"/>
       <c r="F20" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="G20" s="15" t="s">
+        <v>83</v>
+      </c>
+      <c r="H20" s="6"/>
+      <c r="I20" s="19"/>
+    </row>
+    <row r="21" spans="1:9" ht="139.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="7">
+        <v>17</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="E21" s="6"/>
+      <c r="F21" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="G21" s="15" t="s">
+        <v>83</v>
+      </c>
+      <c r="H21" s="6"/>
+      <c r="I21" s="19"/>
+    </row>
+    <row r="22" spans="1:9" ht="139.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="7">
+        <v>18</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="E22" s="6"/>
+      <c r="F22" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="G22" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="H22" s="6"/>
+      <c r="I22" s="19"/>
+    </row>
+    <row r="23" spans="1:9" ht="139.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="7">
+        <v>19</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="E23" s="6"/>
+      <c r="F23" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="G23" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="H23" s="6"/>
+      <c r="I23" s="19"/>
+    </row>
+    <row r="24" spans="1:9" ht="165.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="7">
+        <v>20</v>
+      </c>
+      <c r="B24" s="23" t="s">
+        <v>39</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D24" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="G20" s="19" t="s">
+      <c r="E24" s="6"/>
+      <c r="F24" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="G24" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="H20" s="11"/>
-      <c r="I20" s="30"/>
-    </row>
-    <row r="21" spans="1:9" ht="217.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="12">
+      <c r="H24" s="6"/>
+      <c r="I24" s="19"/>
+    </row>
+    <row r="25" spans="1:9" ht="206.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="7">
+        <v>21</v>
+      </c>
+      <c r="B25" s="23" t="s">
+        <v>40</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="E25" s="6"/>
+      <c r="F25" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="G25" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="B21" s="35" t="s">
-        <v>31</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="D21" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="E21" s="1"/>
-      <c r="F21" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="G21" s="19" t="s">
-        <v>11</v>
-      </c>
-      <c r="H21" s="11"/>
-      <c r="I21" s="30"/>
-    </row>
-    <row r="22" spans="1:9" ht="176.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="12">
-        <v>12</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="D22" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="E22" s="1"/>
-      <c r="F22" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="G22" s="19" t="s">
-        <v>11</v>
-      </c>
-      <c r="H22" s="11"/>
-      <c r="I22" s="30"/>
-    </row>
-    <row r="23" spans="1:9" ht="133.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="12">
-        <v>13</v>
-      </c>
-      <c r="B23" s="37" t="s">
-        <v>37</v>
-      </c>
-      <c r="C23" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="D23" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="E23" s="1"/>
-      <c r="F23" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="G23" s="19" t="s">
-        <v>11</v>
-      </c>
-      <c r="H23" s="11"/>
-      <c r="I23" s="30"/>
-    </row>
-    <row r="24" spans="1:9" ht="149.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="12">
-        <v>14</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="C24" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="D24" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="E24" s="1"/>
-      <c r="F24" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="G24" s="19" t="s">
-        <v>11</v>
-      </c>
-      <c r="H24" s="11"/>
-      <c r="I24" s="30"/>
-    </row>
-    <row r="25" spans="1:9" ht="147.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="12">
-        <v>15</v>
-      </c>
-      <c r="B25" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C25" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="D25" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="E25" s="1"/>
-      <c r="F25" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="G25" s="20" t="s">
-        <v>84</v>
-      </c>
-      <c r="H25" s="11"/>
-      <c r="I25" s="30"/>
-    </row>
-    <row r="26" spans="1:9" ht="139.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="12">
-        <v>16</v>
+      <c r="H25" s="6"/>
+      <c r="I25" s="19"/>
+    </row>
+    <row r="26" spans="1:9" ht="158.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="7">
+        <v>22</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>27</v>
+        <v>41</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>68</v>
+        <v>52</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="E26" s="1"/>
       <c r="F26" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="G26" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="H26" s="6"/>
+      <c r="I26" s="19"/>
+    </row>
+    <row r="27" spans="1:9" ht="135" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="7">
+        <v>23</v>
+      </c>
+      <c r="B27" s="25" t="s">
+        <v>38</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="E27" s="1"/>
+      <c r="F27" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="G27" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="H27" s="6"/>
+      <c r="I27" s="19"/>
+    </row>
+    <row r="28" spans="1:9" ht="131.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="7">
+        <v>24</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="E28" s="1"/>
+      <c r="F28" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="G28" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="H28" s="6"/>
+      <c r="I28" s="19"/>
+    </row>
+    <row r="29" spans="1:9" ht="149.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="7">
+        <v>25</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="E29" s="1"/>
+      <c r="F29" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="G29" s="15" t="s">
+        <v>83</v>
+      </c>
+      <c r="H29" s="7"/>
+      <c r="I29" s="7"/>
+    </row>
+    <row r="30" spans="1:9" ht="139.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="7">
+        <v>26</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="E30" s="1"/>
+      <c r="F30" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="G30" s="15" t="s">
+        <v>83</v>
+      </c>
+      <c r="H30" s="7"/>
+      <c r="I30" s="7"/>
+    </row>
+    <row r="31" spans="1:9" ht="128.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="7">
+        <v>27</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="D31" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="G26" s="20" t="s">
-        <v>84</v>
-      </c>
-      <c r="H26" s="11"/>
-      <c r="I26" s="30"/>
-    </row>
-    <row r="27" spans="1:9" ht="139.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="12">
-        <v>17</v>
-      </c>
-      <c r="B27" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="C27" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="D27" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="E27" s="11"/>
-      <c r="F27" s="1" t="s">
+      <c r="E31" s="6"/>
+      <c r="F31" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="G31" s="15" t="s">
+        <v>83</v>
+      </c>
+      <c r="H31" s="7"/>
+      <c r="I31" s="7"/>
+    </row>
+    <row r="32" spans="1:9" ht="139.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="7">
+        <v>28</v>
+      </c>
+      <c r="B32" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="G27" s="20" t="s">
-        <v>84</v>
-      </c>
-      <c r="H27" s="11"/>
-      <c r="I27" s="30"/>
-    </row>
-    <row r="28" spans="1:9" ht="139.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="12">
-        <v>18</v>
-      </c>
-      <c r="B28" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="C28" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="D28" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="E28" s="11"/>
-      <c r="F28" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="G28" s="19" t="s">
+      <c r="C32" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="E32" s="6"/>
+      <c r="F32" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="G32" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="H28" s="11"/>
-      <c r="I28" s="30"/>
-    </row>
-    <row r="29" spans="1:9" ht="139.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="12">
-        <v>19</v>
-      </c>
-      <c r="B29" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="C29" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="D29" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="E29" s="11"/>
-      <c r="F29" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="G29" s="19" t="s">
+    </row>
+    <row r="33" spans="1:7" ht="89.25" x14ac:dyDescent="0.25">
+      <c r="A33" s="7">
+        <v>29</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="E33" s="6"/>
+      <c r="F33" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="G33" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="H29" s="11"/>
-      <c r="I29" s="30"/>
-    </row>
-    <row r="30" spans="1:9" ht="165.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="12">
-        <v>20</v>
-      </c>
-      <c r="B30" s="35" t="s">
-        <v>40</v>
-      </c>
-      <c r="C30" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="D30" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="E30" s="11"/>
-      <c r="F30" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="G30" s="19" t="s">
+    </row>
+    <row r="34" spans="1:7" ht="147" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="7">
+        <v>30</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="E34" s="6"/>
+      <c r="F34" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="G34" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="H30" s="11"/>
-      <c r="I30" s="30"/>
-    </row>
-    <row r="31" spans="1:9" ht="206.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="12">
-        <v>21</v>
-      </c>
-      <c r="B31" s="35" t="s">
-        <v>41</v>
-      </c>
-      <c r="C31" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="D31" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="E31" s="11"/>
-      <c r="F31" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="G31" s="19" t="s">
-        <v>11</v>
-      </c>
-      <c r="H31" s="11"/>
-      <c r="I31" s="30"/>
-    </row>
-    <row r="32" spans="1:9" ht="158.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="12">
-        <v>22</v>
-      </c>
-      <c r="B32" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="C32" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="D32" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="E32" s="1"/>
-      <c r="F32" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="G32" s="19" t="s">
-        <v>11</v>
-      </c>
-      <c r="H32" s="11"/>
-      <c r="I32" s="30"/>
-    </row>
-    <row r="33" spans="1:9" ht="135" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="12">
-        <v>23</v>
-      </c>
-      <c r="B33" s="37" t="s">
-        <v>39</v>
-      </c>
-      <c r="C33" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="D33" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="E33" s="1"/>
-      <c r="F33" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="G33" s="19" t="s">
-        <v>11</v>
-      </c>
-      <c r="H33" s="11"/>
-      <c r="I33" s="30"/>
-    </row>
-    <row r="34" spans="1:9" ht="131.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="12">
-        <v>24</v>
-      </c>
-      <c r="B34" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="C34" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="D34" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="E34" s="1"/>
-      <c r="F34" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="G34" s="19" t="s">
-        <v>11</v>
-      </c>
-      <c r="H34" s="11"/>
-      <c r="I34" s="30"/>
-    </row>
-    <row r="35" spans="1:9" ht="149.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="12">
-        <v>25</v>
-      </c>
-      <c r="B35" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="C35" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="D35" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="E35" s="1"/>
-      <c r="F35" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="G35" s="20" t="s">
-        <v>84</v>
-      </c>
-      <c r="H35" s="12"/>
-      <c r="I35" s="12"/>
-    </row>
-    <row r="36" spans="1:9" ht="139.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="12">
-        <v>26</v>
-      </c>
-      <c r="B36" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="C36" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="D36" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="E36" s="1"/>
-      <c r="F36" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="G36" s="20" t="s">
-        <v>84</v>
-      </c>
-      <c r="H36" s="12"/>
-      <c r="I36" s="12"/>
-    </row>
-    <row r="37" spans="1:9" ht="128.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="12">
-        <v>27</v>
-      </c>
-      <c r="B37" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="C37" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="D37" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="E37" s="11"/>
-      <c r="F37" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="G37" s="20" t="s">
-        <v>84</v>
-      </c>
-      <c r="H37" s="12"/>
-      <c r="I37" s="12"/>
-    </row>
-    <row r="38" spans="1:9" ht="139.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="12">
-        <v>28</v>
-      </c>
-      <c r="B38" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="C38" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="D38" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="E38" s="11"/>
-      <c r="F38" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="G38" s="19" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="39" spans="1:9" ht="89.25" x14ac:dyDescent="0.25">
-      <c r="A39" s="12">
-        <v>29</v>
-      </c>
-      <c r="B39" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="C39" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="D39" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="E39" s="11"/>
-      <c r="F39" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="G39" s="19" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="40" spans="1:9" ht="147" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="12">
-        <v>30</v>
-      </c>
-      <c r="B40" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="C40" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="D40" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="E40" s="11"/>
-      <c r="F40" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="G40" s="19" t="s">
-        <v>11</v>
-      </c>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="1">
     <mergeCell ref="A1:A2"/>
-    <mergeCell ref="B6:H6"/>
-    <mergeCell ref="B7:H7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>